<commit_message>
Alternative pipeline to parse a file in the unified format and insert it into the db is working. Can test by running DataPipelineTester class.
Modified Line class.

Added methods to the DBLoader class for accessing db, adding new ctegory
to db and adding new metric to the db.

Added method to the DBSaver to save Line object in the db.
</commit_message>
<xml_diff>
--- a/MHTCDashboard/TestUnifiedFile.xlsx
+++ b/MHTCDashboard/TestUnifiedFile.xlsx
@@ -4,36 +4,37 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="150" windowWidth="24915" windowHeight="12075"/>
+    <workbookView xWindow="0" yWindow="2505" windowWidth="18330" windowHeight="6075"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="0"/>
+  <oleSize ref="A1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
-    <t>massachusetts</t>
-  </si>
-  <si>
-    <t>State</t>
-  </si>
-  <si>
-    <t>Year</t>
-  </si>
-  <si>
-    <t>texas</t>
-  </si>
-  <si>
     <t>testing metric name</t>
   </si>
   <si>
     <t>Testing Category Name</t>
+  </si>
+  <si>
+    <t>state</t>
+  </si>
+  <si>
+    <t>year</t>
+  </si>
+  <si>
+    <t>Massachusetts</t>
+  </si>
+  <si>
+    <t>Texas</t>
   </si>
 </sst>
 </file>
@@ -374,7 +375,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -384,23 +387,23 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C2" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="B3">
         <v>9090</v>
@@ -411,7 +414,7 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="B4">
         <v>9090</v>

</xml_diff>

<commit_message>
debugged UnifiedParser and added test case
</commit_message>
<xml_diff>
--- a/MHTCDashboard/TestUnifiedFile.xlsx
+++ b/MHTCDashboard/TestUnifiedFile.xlsx
@@ -12,7 +12,6 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A1"/>
 </workbook>
 </file>
 
@@ -376,7 +375,7 @@
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -406,7 +405,7 @@
         <v>4</v>
       </c>
       <c r="B3">
-        <v>9090</v>
+        <v>1920</v>
       </c>
       <c r="C3">
         <v>11111</v>
@@ -417,7 +416,7 @@
         <v>5</v>
       </c>
       <c r="B4">
-        <v>9090</v>
+        <v>1920</v>
       </c>
       <c r="C4">
         <v>22222</v>

</xml_diff>

<commit_message>
Added a transaction manager to handle uploading multiple data tuples (Lines from one source) into the database. If one line fails, the entire upload will fail.
</commit_message>
<xml_diff>
--- a/MHTCDashboard/TestUnifiedFile.xlsx
+++ b/MHTCDashboard/TestUnifiedFile.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alex Fortier\Documents\mqp\MHTCDashboard\MHTCDashboard\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="2505" windowWidth="18330" windowHeight="6075"/>
   </bookViews>
@@ -16,10 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
-  <si>
-    <t>testing metric name</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="7">
   <si>
     <t>Testing Category Name</t>
   </si>
@@ -34,6 +36,12 @@
   </si>
   <si>
     <t>Texas</t>
+  </si>
+  <si>
+    <t>testmetrica</t>
+  </si>
+  <si>
+    <t>Georgia</t>
   </si>
 </sst>
 </file>
@@ -81,6 +89,9 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
@@ -128,7 +139,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -163,7 +174,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -372,10 +383,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -386,18 +397,18 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
         <v>2</v>
       </c>
-      <c r="B2" t="s">
-        <v>3</v>
-      </c>
       <c r="C2" t="s">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -405,20 +416,42 @@
         <v>4</v>
       </c>
       <c r="B3">
-        <v>1920</v>
+        <v>1983</v>
       </c>
       <c r="C3">
-        <v>11111</v>
+        <v>44444</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B4">
+        <v>1903</v>
+      </c>
+      <c r="C4">
+        <v>55555</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5">
         <v>1920</v>
       </c>
-      <c r="C4">
+      <c r="C5">
+        <v>11111</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6">
+        <v>1920</v>
+      </c>
+      <c r="C6">
         <v>22222</v>
       </c>
     </row>

</xml_diff>